<commit_message>
Addition to last commit
</commit_message>
<xml_diff>
--- a/LabBook/userData.xlsx
+++ b/LabBook/userData.xlsx
@@ -151,7 +151,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>43785.0</v>
+        <v>43788.0</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -216,7 +216,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n" s="2">
-        <v>43785.0</v>
+        <v>43788.0</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -239,7 +239,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>43785.0</v>
+        <v>43788.0</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -289,7 +289,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="n" s="2">
-        <v>43785.334085648145</v>
+        <v>43788.81340277778</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>

</xml_diff>